<commit_message>
Manager + Container + Enums 추가 / DataContainer 생성하는 기능 추가 등
</commit_message>
<xml_diff>
--- a/Assets/Data/Excels/Human.xlsx
+++ b/Assets/Data/Excels/Human.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeonHyun9\Downloads\DataGenerator\Assets\Data\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataGenerator\Assets\Data\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF59BDC9-B20D-4D9F-BF4D-9017CCC2C08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE04BB0D-DD75-41F2-986F-7E5F6383C9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -55,10 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Scores</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -67,10 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1,2,3,4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -84,6 +64,26 @@
   </si>
   <si>
     <t>점수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NameId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Karina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Winter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chawon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kazuha</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,42 +412,42 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -466,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -477,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -488,10 +488,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>